<commit_message>
added the final presentation file
</commit_message>
<xml_diff>
--- a/Statistics/DataCollection.xlsx
+++ b/Statistics/DataCollection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skyla\OneDrive\Desktop\SkyVale_Repo\Statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCD2D75-6354-4DA9-9F82-8199990E76B0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC88AFC-BC59-4D78-9387-FDB828631553}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1EF09E01-2087-1546-9C39-6B7F81A953B7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1EF09E01-2087-1546-9C39-6B7F81A953B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -421,12 +421,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -453,6 +447,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1088,6 +1088,785 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="107"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="7"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Games Sold by Generation (millions)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sold (mil)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent5">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$4:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>31.28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.670000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.61</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8A7D-4384-B691-9F974AAB097D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="-25"/>
+        <c:axId val="11341343"/>
+        <c:axId val="2101029423"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="11341343"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2101029423"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2101029423"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="11341343"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="106"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="6"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Consoles</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Sold (millions)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:shade val="76000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent4">
+                  <a:shade val="76000"/>
+                  <a:satMod val="175000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$H$4:$H$8</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Gameboy/Gameboy Color</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gameboy Advance</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Nintendo DS/Dsi</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Nintendo 3DS/2DS</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Nintendo Switch</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$4:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>118.69</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>81.510000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>154.02000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75.28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36.869999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-82AA-4277-A74A-0594D30B5613}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:overlap val="-50"/>
+        <c:axId val="60751"/>
+        <c:axId val="2101043567"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:spPr>
+                  <a:noFill/>
+                  <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4">
+                        <a:tint val="77000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:miter lim="800000"/>
+                  </a:ln>
+                  <a:effectLst>
+                    <a:glow rad="63500">
+                      <a:schemeClr val="accent4">
+                        <a:tint val="77000"/>
+                        <a:satMod val="175000"/>
+                        <a:alpha val="25000"/>
+                      </a:schemeClr>
+                    </a:glow>
+                  </a:effectLst>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$H$4:$H$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="5"/>
+                      <c:pt idx="0">
+                        <c:v>Gameboy/Gameboy Color</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Gameboy Advance</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Nintendo DS/Dsi</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Nintendo 3DS/2DS</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Nintendo Switch</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$I$4:$I$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="5"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-82AA-4277-A74A-0594D30B5613}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="60751"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2101043567"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2101043567"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="60751"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
@@ -1125,6 +1904,18 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="18">
+  <a:schemeClr val="accent5"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="24">
+  <a:schemeClr val="accent4"/>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="340">
   <cs:axisTitle>
@@ -1622,6 +2413,1105 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="213">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="339">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="10800000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst/>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -1660,6 +3550,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>833437</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>185737</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BCB8AB6-4CBD-46D9-9858-194785A63BEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9903AC33-00C6-4E16-9EF6-95B795751A36}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1967,8 +3929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C170645-77FE-F146-9F98-D104F5BF949F}">
   <dimension ref="A2:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1992,45 +3954,45 @@
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="9"/>
-      <c r="M2" s="39" t="s">
+      <c r="M2" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="41"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="39"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="27"/>
-      <c r="J3" s="28" t="s">
+      <c r="I3" s="41"/>
+      <c r="J3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="K3" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="36" t="s">
+      <c r="M3" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="37" t="s">
+      <c r="N3" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="38" t="s">
+      <c r="O3" s="36" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2098,7 +4060,7 @@
       <c r="N5" s="17">
         <v>39.32</v>
       </c>
-      <c r="O5" s="35">
+      <c r="O5" s="33">
         <v>81.510000000000005</v>
       </c>
     </row>
@@ -2223,19 +4185,19 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="33">
+      <c r="E12" s="31">
         <f>AVERAGE(E4:E10)</f>
         <v>20.702857142857145</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="32">
         <f>STDEV(E4:E10)</f>
         <v>5.8641473216081232</v>
       </c>

</xml_diff>